<commit_message>
feature: make sure that the line lenght is not decreasing during XLSX -> CSV conversion
</commit_message>
<xml_diff>
--- a/tests/data/reader/test-simple.xlsx
+++ b/tests/data/reader/test-simple.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">a</t>
   </si>
@@ -38,6 +38,18 @@
   </si>
   <si>
     <t xml:space="preserve">how are you?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">another</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">present</t>
   </si>
 </sst>
 </file>
@@ -52,6 +64,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -111,8 +124,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -129,11 +146,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
@@ -142,42 +159,63 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>